<commit_message>
Ran ML tests for subject 5. Updated parsed data with subject 5 results.
</commit_message>
<xml_diff>
--- a/ClassifierTesterResults/Individual/OpenBCI/HF-MM-Parsed_Results.xlsx
+++ b/ClassifierTesterResults/Individual/OpenBCI/HF-MM-Parsed_Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="233">
   <si>
     <t>subject_no</t>
   </si>
@@ -154,6 +154,9 @@
     <t>4</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>motor_cortex</t>
   </si>
   <si>
@@ -169,6 +172,9 @@
     <t>0.7810526315789474</t>
   </si>
   <si>
+    <t>0.9263157894736842</t>
+  </si>
+  <si>
     <t>0.49777777777777776</t>
   </si>
   <si>
@@ -181,6 +187,9 @@
     <t>0.7377777777777778</t>
   </si>
   <si>
+    <t>0.9155555555555555</t>
+  </si>
+  <si>
     <t>0.4682900432900433</t>
   </si>
   <si>
@@ -193,6 +202,9 @@
     <t>0.8153030303030304</t>
   </si>
   <si>
+    <t>0.9400000000000001</t>
+  </si>
+  <si>
     <t>0.478030303030303</t>
   </si>
   <si>
@@ -205,6 +217,9 @@
     <t>0.7623099415204677</t>
   </si>
   <si>
+    <t>0.9261300309597523</t>
+  </si>
+  <si>
     <t>0.446</t>
   </si>
   <si>
@@ -217,6 +232,9 @@
     <t>0.887888888888889</t>
   </si>
   <si>
+    <t>0.9611111111111112</t>
+  </si>
+  <si>
     <t>0.5094736842105263</t>
   </si>
   <si>
@@ -229,6 +247,9 @@
     <t>0.853157894736842</t>
   </si>
   <si>
+    <t>0.8957894736842105</t>
+  </si>
+  <si>
     <t>0.47555555555555556</t>
   </si>
   <si>
@@ -250,6 +271,9 @@
     <t>0.8855555555555557</t>
   </si>
   <si>
+    <t>0.8936363636363638</t>
+  </si>
+  <si>
     <t>0.37</t>
   </si>
   <si>
@@ -262,6 +286,9 @@
     <t>0.8456140350877194</t>
   </si>
   <si>
+    <t>0.8986363636363637</t>
+  </si>
+  <si>
     <t>0.5033333333333333</t>
   </si>
   <si>
@@ -274,6 +301,9 @@
     <t>0.8644444444444443</t>
   </si>
   <si>
+    <t>0.9468888888888889</t>
+  </si>
+  <si>
     <t>0.43684210526315786</t>
   </si>
   <si>
@@ -286,6 +316,9 @@
     <t>0.6868421052631579</t>
   </si>
   <si>
+    <t>0.8742105263157894</t>
+  </si>
+  <si>
     <t>0.4</t>
   </si>
   <si>
@@ -298,6 +331,9 @@
     <t>0.5666666666666667</t>
   </si>
   <si>
+    <t>0.7911111111111111</t>
+  </si>
+  <si>
     <t>0.42444444444444446</t>
   </si>
   <si>
@@ -310,6 +346,9 @@
     <t>0.759920634920635</t>
   </si>
   <si>
+    <t>0.96</t>
+  </si>
+  <si>
     <t>0.3997258297258297</t>
   </si>
   <si>
@@ -322,6 +361,9 @@
     <t>0.6398692810457517</t>
   </si>
   <si>
+    <t>0.8573684210526314</t>
+  </si>
+  <si>
     <t>0.43977777777777777</t>
   </si>
   <si>
@@ -334,6 +376,9 @@
     <t>0.8379999999999999</t>
   </si>
   <si>
+    <t>0.9366666666666668</t>
+  </si>
+  <si>
     <t>0.5210526315789474</t>
   </si>
   <si>
@@ -346,6 +391,9 @@
     <t>0.8231578947368421</t>
   </si>
   <si>
+    <t>0.8442105263157895</t>
+  </si>
+  <si>
     <t>0.8755555555555556</t>
   </si>
   <si>
@@ -358,6 +406,9 @@
     <t>0.6977777777777778</t>
   </si>
   <si>
+    <t>0.6888888888888889</t>
+  </si>
+  <si>
     <t>0.5117156862745098</t>
   </si>
   <si>
@@ -370,6 +421,9 @@
     <t>0.9577777777777777</t>
   </si>
   <si>
+    <t>1.0</t>
+  </si>
+  <si>
     <t>0.6452380952380954</t>
   </si>
   <si>
@@ -382,6 +436,9 @@
     <t>0.7815371762740184</t>
   </si>
   <si>
+    <t>0.8144117647058822</t>
+  </si>
+  <si>
     <t>0.5199999999999999</t>
   </si>
   <si>
@@ -394,6 +451,9 @@
     <t>0.8613333333333333</t>
   </si>
   <si>
+    <t>0.7375555555555555</t>
+  </si>
+  <si>
     <t>0.5626315789473685</t>
   </si>
   <si>
@@ -412,12 +472,12 @@
     <t>0.8044444444444444</t>
   </si>
   <si>
-    <t>0.9155555555555555</t>
-  </si>
-  <si>
     <t>0.8977777777777778</t>
   </si>
   <si>
+    <t>0.7733333333333332</t>
+  </si>
+  <si>
     <t>0.5642857142857143</t>
   </si>
   <si>
@@ -430,6 +490,9 @@
     <t>0.8703030303030304</t>
   </si>
   <si>
+    <t>0.8742063492063492</t>
+  </si>
+  <si>
     <t>0.6060193236714976</t>
   </si>
   <si>
@@ -442,6 +505,9 @@
     <t>0.8758473724417997</t>
   </si>
   <si>
+    <t>0.8131461675579322</t>
+  </si>
+  <si>
     <t>0.4966666666666667</t>
   </si>
   <si>
@@ -454,6 +520,9 @@
     <t>0.9617777777777778</t>
   </si>
   <si>
+    <t>0.9284444444444444</t>
+  </si>
+  <si>
     <t>0.6963157894736842</t>
   </si>
   <si>
@@ -463,6 +532,9 @@
     <t>0.7084210526315788</t>
   </si>
   <si>
+    <t>0.7699999999999999</t>
+  </si>
+  <si>
     <t>0.6444444444444444</t>
   </si>
   <si>
@@ -475,6 +547,9 @@
     <t>0.6733333333333333</t>
   </si>
   <si>
+    <t>0.7511111111111111</t>
+  </si>
+  <si>
     <t>0.5075757575757576</t>
   </si>
   <si>
@@ -487,6 +562,9 @@
     <t>0.732034632034632</t>
   </si>
   <si>
+    <t>0.8051282051282052</t>
+  </si>
+  <si>
     <t>0.5673160173160173</t>
   </si>
   <si>
@@ -499,6 +577,9 @@
     <t>0.6895975232198143</t>
   </si>
   <si>
+    <t>0.7691120384080404</t>
+  </si>
+  <si>
     <t>0.5</t>
   </si>
   <si>
@@ -511,6 +592,9 @@
     <t>0.8033333333333333</t>
   </si>
   <si>
+    <t>0.844</t>
+  </si>
+  <si>
     <t>0.5210526315789473</t>
   </si>
   <si>
@@ -529,6 +613,9 @@
     <t>0.7</t>
   </si>
   <si>
+    <t>0.7711111111111111</t>
+  </si>
+  <si>
     <t>0.5195804195804196</t>
   </si>
   <si>
@@ -541,6 +628,9 @@
     <t>0.8246464646464646</t>
   </si>
   <si>
+    <t>0.7829059829059829</t>
+  </si>
+  <si>
     <t>0.5743290043290042</t>
   </si>
   <si>
@@ -553,6 +643,9 @@
     <t>0.7587409700722394</t>
   </si>
   <si>
+    <t>0.7728272086866783</t>
+  </si>
+  <si>
     <t>0.44866666666666666</t>
   </si>
   <si>
@@ -565,6 +658,9 @@
     <t>0.8504444444444446</t>
   </si>
   <si>
+    <t>0.8351111111111111</t>
+  </si>
+  <si>
     <t>0.7089473684210527</t>
   </si>
   <si>
@@ -574,7 +670,7 @@
     <t>0.9689473684210526</t>
   </si>
   <si>
-    <t>1.0</t>
+    <t>0.9694736842105263</t>
   </si>
   <si>
     <t>0.5844444444444445</t>
@@ -604,6 +700,9 @@
     <t>0.9691876750700279</t>
   </si>
   <si>
+    <t>0.9682539682539684</t>
+  </si>
+  <si>
     <t>0.704</t>
   </si>
   <si>
@@ -611,6 +710,9 @@
   </si>
   <si>
     <t>0.9935555555555556</t>
+  </si>
+  <si>
+    <t>0.9879999999999999</t>
   </si>
 </sst>
 </file>
@@ -968,7 +1070,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AQ5"/>
+  <dimension ref="A1:AQ6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1110,127 +1212,127 @@
         <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="I2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="J2" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="K2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="L2" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="M2" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="N2" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="O2" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="P2" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="Q2" t="s">
+        <v>111</v>
+      </c>
+      <c r="R2" t="s">
+        <v>116</v>
+      </c>
+      <c r="S2" t="s">
+        <v>121</v>
+      </c>
+      <c r="T2" t="s">
+        <v>126</v>
+      </c>
+      <c r="U2" t="s">
+        <v>131</v>
+      </c>
+      <c r="V2" t="s">
+        <v>136</v>
+      </c>
+      <c r="W2" t="s">
+        <v>141</v>
+      </c>
+      <c r="X2" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>164</v>
+      </c>
+      <c r="AC2" t="s">
         <v>98</v>
       </c>
-      <c r="R2" t="s">
-        <v>102</v>
-      </c>
-      <c r="S2" t="s">
-        <v>106</v>
-      </c>
-      <c r="T2" t="s">
-        <v>110</v>
-      </c>
-      <c r="U2" t="s">
-        <v>114</v>
-      </c>
-      <c r="V2" t="s">
-        <v>118</v>
-      </c>
-      <c r="W2" t="s">
-        <v>122</v>
-      </c>
-      <c r="X2" t="s">
-        <v>126</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>130</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>134</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>138</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>142</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>88</v>
-      </c>
       <c r="AD2" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
       <c r="AE2" t="s">
-        <v>153</v>
+        <v>178</v>
       </c>
       <c r="AF2" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
       <c r="AG2" t="s">
-        <v>161</v>
+        <v>188</v>
       </c>
       <c r="AH2" t="s">
-        <v>165</v>
+        <v>193</v>
       </c>
       <c r="AI2" t="s">
-        <v>169</v>
+        <v>197</v>
       </c>
       <c r="AJ2" t="s">
-        <v>171</v>
+        <v>200</v>
       </c>
       <c r="AK2" t="s">
-        <v>175</v>
+        <v>205</v>
       </c>
       <c r="AL2" t="s">
-        <v>179</v>
+        <v>210</v>
       </c>
       <c r="AM2" t="s">
-        <v>183</v>
+        <v>215</v>
       </c>
       <c r="AN2" t="s">
-        <v>187</v>
+        <v>219</v>
       </c>
       <c r="AO2" t="s">
-        <v>190</v>
+        <v>222</v>
       </c>
       <c r="AP2" t="s">
-        <v>193</v>
+        <v>225</v>
       </c>
       <c r="AQ2" t="s">
-        <v>196</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -1241,127 +1343,127 @@
         <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="J3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K3" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="L3" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="M3" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="N3" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="O3" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="P3" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="Q3" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="R3" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="S3" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="T3" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="U3" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="V3" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="W3" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="X3" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="Y3" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
       <c r="Z3" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="AA3" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="AB3" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="AC3" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="AD3" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="AE3" t="s">
-        <v>154</v>
+        <v>179</v>
       </c>
       <c r="AF3" t="s">
-        <v>158</v>
+        <v>184</v>
       </c>
       <c r="AG3" t="s">
-        <v>162</v>
+        <v>189</v>
       </c>
       <c r="AH3" t="s">
-        <v>166</v>
+        <v>194</v>
       </c>
       <c r="AI3" t="s">
-        <v>170</v>
+        <v>198</v>
       </c>
       <c r="AJ3" t="s">
-        <v>172</v>
+        <v>201</v>
       </c>
       <c r="AK3" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="AL3" t="s">
-        <v>180</v>
+        <v>211</v>
       </c>
       <c r="AM3" t="s">
-        <v>184</v>
+        <v>216</v>
       </c>
       <c r="AN3" t="s">
-        <v>188</v>
+        <v>220</v>
       </c>
       <c r="AO3" t="s">
-        <v>191</v>
+        <v>223</v>
       </c>
       <c r="AP3" t="s">
-        <v>194</v>
+        <v>226</v>
       </c>
       <c r="AQ3" t="s">
-        <v>197</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -1372,127 +1474,127 @@
         <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I4" t="s">
+        <v>75</v>
+      </c>
+      <c r="J4" t="s">
+        <v>79</v>
+      </c>
+      <c r="K4" t="s">
+        <v>83</v>
+      </c>
+      <c r="L4" t="s">
+        <v>88</v>
+      </c>
+      <c r="M4" t="s">
+        <v>93</v>
+      </c>
+      <c r="N4" t="s">
+        <v>98</v>
+      </c>
+      <c r="O4" t="s">
+        <v>103</v>
+      </c>
+      <c r="P4" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>113</v>
+      </c>
+      <c r="R4" t="s">
+        <v>118</v>
+      </c>
+      <c r="S4" t="s">
+        <v>123</v>
+      </c>
+      <c r="T4" t="s">
+        <v>128</v>
+      </c>
+      <c r="U4" t="s">
+        <v>133</v>
+      </c>
+      <c r="V4" t="s">
+        <v>138</v>
+      </c>
+      <c r="W4" t="s">
+        <v>143</v>
+      </c>
+      <c r="X4" t="s">
+        <v>148</v>
+      </c>
+      <c r="Y4" t="s">
         <v>57</v>
       </c>
-      <c r="G4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" t="s">
-        <v>65</v>
-      </c>
-      <c r="I4" t="s">
-        <v>69</v>
-      </c>
-      <c r="J4" t="s">
-        <v>72</v>
-      </c>
-      <c r="K4" t="s">
-        <v>76</v>
-      </c>
-      <c r="L4" t="s">
-        <v>80</v>
-      </c>
-      <c r="M4" t="s">
-        <v>84</v>
-      </c>
-      <c r="N4" t="s">
-        <v>88</v>
-      </c>
-      <c r="O4" t="s">
-        <v>92</v>
-      </c>
-      <c r="P4" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>100</v>
-      </c>
-      <c r="R4" t="s">
-        <v>104</v>
-      </c>
-      <c r="S4" t="s">
-        <v>108</v>
-      </c>
-      <c r="T4" t="s">
-        <v>112</v>
-      </c>
-      <c r="U4" t="s">
-        <v>116</v>
-      </c>
-      <c r="V4" t="s">
-        <v>120</v>
-      </c>
-      <c r="W4" t="s">
-        <v>124</v>
-      </c>
-      <c r="X4" t="s">
-        <v>128</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>132</v>
-      </c>
       <c r="Z4" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="AA4" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="AB4" t="s">
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="AC4" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="AD4" t="s">
-        <v>151</v>
+        <v>175</v>
       </c>
       <c r="AE4" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="AF4" t="s">
-        <v>159</v>
+        <v>185</v>
       </c>
       <c r="AG4" t="s">
-        <v>163</v>
+        <v>190</v>
       </c>
       <c r="AH4" t="s">
-        <v>167</v>
+        <v>195</v>
       </c>
       <c r="AI4" t="s">
-        <v>151</v>
+        <v>175</v>
       </c>
       <c r="AJ4" t="s">
-        <v>173</v>
+        <v>202</v>
       </c>
       <c r="AK4" t="s">
-        <v>177</v>
+        <v>207</v>
       </c>
       <c r="AL4" t="s">
-        <v>181</v>
+        <v>212</v>
       </c>
       <c r="AM4" t="s">
-        <v>185</v>
+        <v>217</v>
       </c>
       <c r="AN4" t="s">
-        <v>189</v>
+        <v>221</v>
       </c>
       <c r="AO4" t="s">
-        <v>192</v>
+        <v>224</v>
       </c>
       <c r="AP4" t="s">
-        <v>195</v>
+        <v>227</v>
       </c>
       <c r="AQ4" t="s">
-        <v>198</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:43">
@@ -1503,127 +1605,258 @@
         <v>45</v>
       </c>
       <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" t="s">
+        <v>71</v>
+      </c>
+      <c r="I5" t="s">
+        <v>76</v>
+      </c>
+      <c r="J5" t="s">
+        <v>80</v>
+      </c>
+      <c r="K5" t="s">
+        <v>84</v>
+      </c>
+      <c r="L5" t="s">
+        <v>89</v>
+      </c>
+      <c r="M5" t="s">
+        <v>94</v>
+      </c>
+      <c r="N5" t="s">
+        <v>99</v>
+      </c>
+      <c r="O5" t="s">
+        <v>104</v>
+      </c>
+      <c r="P5" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>114</v>
+      </c>
+      <c r="R5" t="s">
+        <v>119</v>
+      </c>
+      <c r="S5" t="s">
+        <v>124</v>
+      </c>
+      <c r="T5" t="s">
+        <v>129</v>
+      </c>
+      <c r="U5" t="s">
+        <v>134</v>
+      </c>
+      <c r="V5" t="s">
+        <v>139</v>
+      </c>
+      <c r="W5" t="s">
+        <v>144</v>
+      </c>
+      <c r="X5" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>167</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>171</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>176</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>181</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>191</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>196</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>203</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>208</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>213</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>135</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>135</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>135</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>135</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>46</v>
       </c>
-      <c r="D5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" t="s">
         <v>62</v>
       </c>
-      <c r="H5" t="s">
-        <v>66</v>
-      </c>
-      <c r="I5" t="s">
-        <v>70</v>
-      </c>
-      <c r="J5" t="s">
-        <v>73</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="G6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" t="s">
         <v>77</v>
       </c>
-      <c r="L5" t="s">
-        <v>81</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="J6" t="s">
+        <v>57</v>
+      </c>
+      <c r="K6" t="s">
         <v>85</v>
       </c>
-      <c r="N5" t="s">
-        <v>89</v>
-      </c>
-      <c r="O5" t="s">
-        <v>93</v>
-      </c>
-      <c r="P5" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>101</v>
-      </c>
-      <c r="R5" t="s">
+      <c r="L6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M6" t="s">
+        <v>95</v>
+      </c>
+      <c r="N6" t="s">
+        <v>100</v>
+      </c>
+      <c r="O6" t="s">
         <v>105</v>
       </c>
-      <c r="S5" t="s">
-        <v>109</v>
-      </c>
-      <c r="T5" t="s">
-        <v>113</v>
-      </c>
-      <c r="U5" t="s">
-        <v>117</v>
-      </c>
-      <c r="V5" t="s">
-        <v>121</v>
-      </c>
-      <c r="W5" t="s">
+      <c r="P6" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>115</v>
+      </c>
+      <c r="R6" t="s">
+        <v>120</v>
+      </c>
+      <c r="S6" t="s">
         <v>125</v>
       </c>
-      <c r="X5" t="s">
-        <v>129</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>133</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>137</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>141</v>
-      </c>
-      <c r="AB5" t="s">
+      <c r="T6" t="s">
+        <v>130</v>
+      </c>
+      <c r="U6" t="s">
+        <v>135</v>
+      </c>
+      <c r="V6" t="s">
+        <v>140</v>
+      </c>
+      <c r="W6" t="s">
         <v>145</v>
       </c>
-      <c r="AC5" t="s">
-        <v>148</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>152</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>156</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>164</v>
-      </c>
-      <c r="AH5" t="s">
+      <c r="X6" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>153</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>163</v>
+      </c>
+      <c r="AB6" t="s">
         <v>168</v>
       </c>
-      <c r="AI5" t="s">
-        <v>54</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>174</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>178</v>
-      </c>
-      <c r="AL5" t="s">
+      <c r="AC6" t="s">
+        <v>172</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>177</v>
+      </c>
+      <c r="AE6" t="s">
         <v>182</v>
       </c>
-      <c r="AM5" t="s">
-        <v>186</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>186</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>186</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>186</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>186</v>
+      <c r="AF6" t="s">
+        <v>187</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>192</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>172</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>199</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>204</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>209</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>214</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>218</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>223</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>228</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>